<commit_message>
add more missing data to spotify data
</commit_message>
<xml_diff>
--- a/data/spotify.xlsx
+++ b/data/spotify.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minedogucu/Desktop/ids-website/slides/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minedogucu/Desktop/stats6-slides/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD79B09-A330-BA41-A74A-AB91B6047D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4737B9-A288-804E-B11D-0A18C057B829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="5840" windowWidth="17860" windowHeight="17440" activeTab="2" xr2:uid="{1BFC579D-EFA7-7C4A-A08D-565DD83982A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{1BFC579D-EFA7-7C4A-A08D-565DD83982A2}"/>
   </bookViews>
   <sheets>
     <sheet name="artist" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2146D6F1-CE58-794C-8112-D7D373818156}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,14 +498,6 @@
         <v>51807131</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>50252529</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -516,7 +508,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA0E7A0-37F1-3B45-88E1-2A4ADC58BC07}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>